<commit_message>
Custom voting classifier results
</commit_message>
<xml_diff>
--- a/presentation/final/KDDM2-Results.xlsx
+++ b/presentation/final/KDDM2-Results.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27217"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/r4ll3/TU Graz/Aktuelles Semester/Knowledge Discovery &amp; Data Mining 2/Project/MLSE/presentation/final/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="116">
   <si>
     <t>Model</t>
   </si>
@@ -399,6 +407,30 @@
   </si>
   <si>
     <t>0.199</t>
+  </si>
+  <si>
+    <t>CustomVotingClassifier(clfs=[OneVsRestClassifier(estimator=MultinomialNB(alpha=0.01, class_prior=None, fit_prior=True),
+          n_jobs=1), OneVsRestClassifier(estimator=KNeighborsClassifier(algorithm='auto', leaf_size=30, metric='minkowski',
+           metric_params=None, n_jobs=1, n_neighbors=10, p=2,
+           weight...obability=True, random_state=None, shrinking=True,
+  tol=0.001, verbose=False),
+          n_jobs=1)],
+            weights=[0.3, 0.3, 0.4])</t>
+  </si>
+  <si>
+    <t>0.461</t>
+  </si>
+  <si>
+    <t>0.428</t>
+  </si>
+  <si>
+    <t>0.253</t>
+  </si>
+  <si>
+    <t>0.296</t>
+  </si>
+  <si>
+    <t>0.499</t>
   </si>
 </sst>
 </file>
@@ -467,12 +499,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -591,15 +629,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -626,9 +661,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -637,116 +669,148 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="105">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1072,693 +1136,729 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.6640625" style="2" customWidth="1"/>
-    <col min="2" max="3" width="10.83203125" style="4"/>
-    <col min="4" max="4" width="17" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="56.1640625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="13.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.33203125" style="2" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="3"/>
+    <col min="4" max="4" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="56.1640625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" ht="60">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="17">
         <v>13669</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="17">
         <v>1614</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="17">
         <v>5</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="17">
         <v>2</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="45">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="16">
         <v>13669</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="16">
         <v>1614</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="16">
         <v>5</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="17">
         <v>2</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30">
+    <row r="4" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>13669</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>1614</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>5</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>2</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>13669</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>1614</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>5</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>2</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="16" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>13669</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>1614</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>5</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>2</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="16">
         <v>13669</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="16">
         <v>1614</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="16">
         <v>5</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="17">
         <v>2</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="M7" s="17" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="30">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="17">
         <v>13669</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="17">
         <v>1614</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="17">
         <v>5</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="17">
         <v>2</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="17" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>13669</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>1614</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>5</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>2</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="16" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="5"/>
     </row>
-    <row r="12" spans="1:13" ht="30">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="17">
         <v>38315</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="17">
         <v>1614</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="17">
         <v>5</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="17">
         <v>2</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J12" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="L12" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="M12" s="17" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="30">
-      <c r="A13" s="12" t="s">
+    <row r="13" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="16">
         <v>38315</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="17">
         <v>1614</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="17">
         <v>5</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="17">
         <v>2</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J13" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="L13" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="M13" s="17" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="30">
-      <c r="A14" s="12" t="s">
+    <row r="14" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="16">
         <v>38315</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="16">
         <v>1614</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="17">
         <v>5</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="17">
         <v>2</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J14" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="L14" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="M14" s="17" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="30">
-      <c r="A15" s="12" t="s">
+    <row r="15" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="16">
         <v>38315</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="16">
         <v>1614</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="17">
         <v>5</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="17">
         <v>2</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="J15" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="L15" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="M15" s="4" t="s">
+      <c r="M15" s="17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>13669</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>1614</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>5</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>2</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="J16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="L16" s="4" t="s">
+      <c r="L16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="M16" s="4" t="s">
+      <c r="M16" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="30">
-      <c r="A17" s="12" t="s">
+    <row r="17" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="16">
         <v>38315</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="17">
         <v>1614</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="17">
         <v>5</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="17">
         <v>2</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="L17" s="4" t="s">
+      <c r="L17" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="M17" s="4" t="s">
+      <c r="M17" s="17" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="30">
-      <c r="A18" s="12" t="s">
+    <row r="18" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="16">
         <v>38315</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="17">
         <v>1614</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="17">
         <v>5</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="17">
         <v>2</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="L18" s="4" t="s">
+      <c r="L18" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="M18" s="4" t="s">
+      <c r="M18" s="17" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="14" t="s">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="3">
         <v>38315</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <v>1614</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="3">
         <v>5</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="3">
         <v>2</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="15" t="s">
+      <c r="H19" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="I19" s="15" t="s">
+      <c r="I19" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="J19" s="15" t="s">
+      <c r="J19" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="K19" s="15" t="s">
+      <c r="K19" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="L19" s="15" t="s">
+      <c r="L19" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="M19" s="15" t="s">
+      <c r="M19" s="13" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="192" x14ac:dyDescent="0.2">
+      <c r="A20" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" s="17">
+        <v>9375</v>
+      </c>
+      <c r="C20" s="17">
+        <v>1614</v>
+      </c>
+      <c r="D20" s="17">
+        <v>5</v>
+      </c>
+      <c r="E20" s="17">
+        <v>2</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="J20" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="K20" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="L20" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="M20" s="17" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Linear SVM numeric results
</commit_message>
<xml_diff>
--- a/presentation/final/KDDM2-Results.xlsx
+++ b/presentation/final/KDDM2-Results.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27217"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/r4ll3/TU Graz/Aktuelles Semester/Knowledge Discovery &amp; Data Mining 2/Project/MLSE/presentation/final/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="122">
   <si>
     <t>Model</t>
   </si>
@@ -431,6 +426,24 @@
   </si>
   <si>
     <t>0.499</t>
+  </si>
+  <si>
+    <t>0.779</t>
+  </si>
+  <si>
+    <t>0.617</t>
+  </si>
+  <si>
+    <t>0.675</t>
+  </si>
+  <si>
+    <t>0.534</t>
+  </si>
+  <si>
+    <t>0.723</t>
+  </si>
+  <si>
+    <t>0.559</t>
   </si>
 </sst>
 </file>
@@ -629,7 +642,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -696,113 +709,116 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="105">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1138,11 +1154,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="51.33203125" style="2" customWidth="1"/>
     <col min="2" max="3" width="10.83203125" style="3"/>
@@ -1158,7 +1174,7 @@
     <col min="13" max="13" width="8.83203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1199,7 +1215,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="64">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -1240,7 +1256,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="48">
       <c r="A3" s="20" t="s">
         <v>21</v>
       </c>
@@ -1281,7 +1297,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="32">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -1322,7 +1338,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -1363,7 +1379,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="A6" s="14" t="s">
         <v>46</v>
       </c>
@@ -1385,8 +1401,26 @@
       <c r="G6" s="7" t="s">
         <v>47</v>
       </c>
+      <c r="H6" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="I6" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="J6" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="K6" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="L6" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="M6" s="24" t="s">
+        <v>121</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13">
       <c r="A7" s="15" t="s">
         <v>46</v>
       </c>
@@ -1427,7 +1461,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="32">
       <c r="A8" s="20" t="s">
         <v>102</v>
       </c>
@@ -1468,7 +1502,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13">
       <c r="A9" s="11" t="s">
         <v>102</v>
       </c>
@@ -1488,13 +1522,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="A10" s="14" t="s">
         <v>108</v>
       </c>
       <c r="B10" s="5"/>
     </row>
-    <row r="12" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="32">
       <c r="A12" s="20" t="s">
         <v>50</v>
       </c>
@@ -1535,7 +1569,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="32">
       <c r="A13" s="15" t="s">
         <v>58</v>
       </c>
@@ -1576,7 +1610,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="32">
       <c r="A14" s="15" t="s">
         <v>65</v>
       </c>
@@ -1617,7 +1651,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="32">
       <c r="A15" s="15" t="s">
         <v>73</v>
       </c>
@@ -1658,7 +1692,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13">
       <c r="A16" s="2" t="s">
         <v>72</v>
       </c>
@@ -1696,7 +1730,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="32">
       <c r="A17" s="15" t="s">
         <v>78</v>
       </c>
@@ -1737,7 +1771,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="32">
       <c r="A18" s="15" t="s">
         <v>85</v>
       </c>
@@ -1778,7 +1812,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" s="12" t="s">
         <v>91</v>
       </c>
@@ -1816,7 +1850,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="192" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="192">
       <c r="A20" s="23" t="s">
         <v>110</v>
       </c>
@@ -1860,5 +1894,10 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Minor presentation and result changes
</commit_message>
<xml_diff>
--- a/presentation/final/KDDM2-Results.xlsx
+++ b/presentation/final/KDDM2-Results.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27217"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/r4ll3/TU Graz/Aktuelles Semester/Knowledge Discovery &amp; Data Mining 2/Project/MLSE/presentation/final/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="820" yWindow="460" windowWidth="27980" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="127">
   <si>
     <t>Model</t>
   </si>
@@ -475,7 +470,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -544,6 +539,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -568,7 +568,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="105">
+  <cellStyleXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -674,8 +674,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -760,113 +764,120 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="105">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="109">
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1202,11 +1213,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="51.33203125" style="2" customWidth="1"/>
     <col min="2" max="3" width="10.83203125" style="3"/>
@@ -1222,7 +1233,7 @@
     <col min="13" max="13" width="8.83203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1263,7 +1274,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="60">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -1304,7 +1315,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="45">
       <c r="A3" s="20" t="s">
         <v>21</v>
       </c>
@@ -1345,7 +1356,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="30">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -1386,7 +1397,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -1427,8 +1438,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:13">
+      <c r="A6" s="30" t="s">
         <v>46</v>
       </c>
       <c r="B6" s="5">
@@ -1468,7 +1479,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13">
       <c r="A7" s="15" t="s">
         <v>46</v>
       </c>
@@ -1509,7 +1520,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="30">
       <c r="A8" s="20" t="s">
         <v>102</v>
       </c>
@@ -1550,7 +1561,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13">
       <c r="A9" s="11" t="s">
         <v>102</v>
       </c>
@@ -1570,13 +1581,27 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="A10" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="5"/>
-    </row>
-    <row r="11" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="B10" s="5">
+        <v>13669</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1614</v>
+      </c>
+      <c r="D10" s="3">
+        <v>5</v>
+      </c>
+      <c r="E10" s="3">
+        <v>2</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="30">
       <c r="A11" s="27" t="s">
         <v>108</v>
       </c>
@@ -1597,7 +1622,7 @@
       <c r="L11" s="17"/>
       <c r="M11" s="17"/>
     </row>
-    <row r="12" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="30">
       <c r="A12" s="20" t="s">
         <v>50</v>
       </c>
@@ -1638,7 +1663,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="30">
       <c r="A13" s="15" t="s">
         <v>58</v>
       </c>
@@ -1679,7 +1704,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="30">
       <c r="A14" s="15" t="s">
         <v>65</v>
       </c>
@@ -1720,7 +1745,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="30">
       <c r="A15" s="15" t="s">
         <v>73</v>
       </c>
@@ -1761,7 +1786,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13">
       <c r="A16" s="2" t="s">
         <v>72</v>
       </c>
@@ -1799,7 +1824,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="30">
       <c r="A17" s="15" t="s">
         <v>78</v>
       </c>
@@ -1840,7 +1865,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="30">
       <c r="A18" s="15" t="s">
         <v>85</v>
       </c>
@@ -1881,7 +1906,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" s="12" t="s">
         <v>91</v>
       </c>
@@ -1919,7 +1944,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="192" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="180">
       <c r="A20" s="23" t="s">
         <v>110</v>
       </c>
@@ -1960,7 +1985,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="256" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="240">
       <c r="A21" s="23" t="s">
         <v>116</v>
       </c>
@@ -2001,7 +2026,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="92" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="89">
       <c r="A22" s="29" t="s">
         <v>126</v>
       </c>
@@ -2009,5 +2034,10 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added KNN numeric results
</commit_message>
<xml_diff>
--- a/presentation/final/KDDM2-Results.xlsx
+++ b/presentation/final/KDDM2-Results.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27217"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/r4ll3/TU Graz/Aktuelles Semester/Knowledge Discovery &amp; Data Mining 2/Project/MLSE/presentation/final/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="780" yWindow="460" windowWidth="28020" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="144">
   <si>
     <t>Model</t>
   </si>
@@ -517,6 +512,15 @@
   </si>
   <si>
     <t>OneVsRestClassifier(MultinomialNB(alpha=0.01))</t>
+  </si>
+  <si>
+    <t>0.512</t>
+  </si>
+  <si>
+    <t>0.270</t>
+  </si>
+  <si>
+    <t>0.269</t>
   </si>
 </sst>
 </file>
@@ -830,129 +834,129 @@
     </xf>
   </cellXfs>
   <cellStyles count="123">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1288,9 +1292,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="51.33203125" style="2" customWidth="1"/>
     <col min="2" max="3" width="10.83203125" style="3"/>
@@ -1306,7 +1312,7 @@
     <col min="13" max="13" width="8.83203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1347,7 +1353,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="64">
       <c r="A2" s="19" t="s">
         <v>11</v>
       </c>
@@ -1388,7 +1394,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="48">
       <c r="A3" s="19" t="s">
         <v>21</v>
       </c>
@@ -1429,7 +1435,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="32">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -1470,7 +1476,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -1511,7 +1517,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="A6" s="28" t="s">
         <v>46</v>
       </c>
@@ -1552,7 +1558,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13">
       <c r="A7" s="14" t="s">
         <v>46</v>
       </c>
@@ -1593,7 +1599,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="32">
       <c r="A8" s="19" t="s">
         <v>101</v>
       </c>
@@ -1634,12 +1640,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13">
       <c r="A9" s="11" t="s">
         <v>101</v>
       </c>
       <c r="B9" s="5">
-        <v>13669</v>
+        <v>1766</v>
       </c>
       <c r="C9" s="3">
         <v>1614</v>
@@ -1653,8 +1659,26 @@
       <c r="F9" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="H9" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>100</v>
+      </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="A10" s="28" t="s">
         <v>107</v>
       </c>
@@ -1695,7 +1719,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="160" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="160">
       <c r="A11" s="21" t="s">
         <v>131</v>
       </c>
@@ -1736,7 +1760,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="32">
       <c r="A12" s="19" t="s">
         <v>50</v>
       </c>
@@ -1777,7 +1801,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="32">
       <c r="A13" s="14" t="s">
         <v>58</v>
       </c>
@@ -1818,7 +1842,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="32">
       <c r="A14" s="14" t="s">
         <v>65</v>
       </c>
@@ -1859,7 +1883,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="32">
       <c r="A15" s="14" t="s">
         <v>73</v>
       </c>
@@ -1900,7 +1924,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13">
       <c r="A16" s="2" t="s">
         <v>72</v>
       </c>
@@ -1938,7 +1962,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="32">
       <c r="A17" s="14" t="s">
         <v>78</v>
       </c>
@@ -1979,7 +2003,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="32">
       <c r="A18" s="14" t="s">
         <v>140</v>
       </c>
@@ -2020,7 +2044,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" s="12" t="s">
         <v>90</v>
       </c>
@@ -2058,7 +2082,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="192" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="192">
       <c r="A20" s="22" t="s">
         <v>109</v>
       </c>
@@ -2099,7 +2123,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="256" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="256">
       <c r="A21" s="22" t="s">
         <v>115</v>
       </c>
@@ -2140,7 +2164,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="92" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="92">
       <c r="A22" s="27" t="s">
         <v>132</v>
       </c>
@@ -2148,5 +2172,10 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>